<commit_message>
add importacion de ruta dinamica, add diseño de las columnas del excel dinamicamente
</commit_message>
<xml_diff>
--- a/processed/datos.xlsx
+++ b/processed/datos.xlsx
@@ -55,10 +55,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,6 +435,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="55" customWidth="1" min="5" max="5"/>
+    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -476,23 +488,22 @@
           <t>Oficio Circular No. 349-2024.pdf</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
           <t>SGTIC/SP/Peren</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>INFORMANDO CREACION DEL DEPARTAMENTO DE COORDINACION DE POLICIA COMUNITARIA.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>ITISIENno de seccionDE PERSONAL YE - Gobermnación S-EDRECCIÓN GENERAL DE TECNOLOGIAS DE L »</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>28 de junio de 2024</t>

</xml_diff>